<commit_message>
add requirement lxml, clear excel with initial update
</commit_message>
<xml_diff>
--- a/EZDC.xlsx
+++ b/EZDC.xlsx
@@ -1189,7 +1189,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1241,22 +1241,18 @@
     </row>
     <row r="2">
       <c r="A2" s="8" t="n">
-        <v>44309.6223059774</v>
+        <v>44309.69303853926</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
           <t>B088RG7N5D</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>CHECKED EMPTY</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>CHECKED EMPTY</t>
-        </is>
+      <c r="C2" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="D2" t="n">
+        <v>237</v>
       </c>
       <c r="E2" t="n">
         <v>54725</v>
@@ -1270,102 +1266,6 @@
         <v>367</v>
       </c>
       <c r="H2" t="inlineStr">
-        <is>
-          <t>Serving Trays</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="8" t="n">
-        <v>44309.62367587614</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>B088RG7N5D</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>4.6</v>
-      </c>
-      <c r="D3" t="n">
-        <v>237</v>
-      </c>
-      <c r="E3" t="n">
-        <v>54725</v>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Kitchen &amp; Dining</t>
-        </is>
-      </c>
-      <c r="G3" t="n">
-        <v>367</v>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>Serving Trays</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="8" t="n">
-        <v>44309.62840518814</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>B088RG7N5D</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>4.6</v>
-      </c>
-      <c r="D4" t="n">
-        <v>237</v>
-      </c>
-      <c r="E4" t="n">
-        <v>54725</v>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Kitchen &amp; Dining</t>
-        </is>
-      </c>
-      <c r="G4" t="n">
-        <v>367</v>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>Serving Trays</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="8" t="n">
-        <v>44309.63153313466</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>B088RG7N5D</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>4.6</v>
-      </c>
-      <c r="D5" t="n">
-        <v>237</v>
-      </c>
-      <c r="E5" t="n">
-        <v>54725</v>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>Kitchen &amp; Dining</t>
-        </is>
-      </c>
-      <c r="G5" t="n">
-        <v>367</v>
-      </c>
-      <c r="H5" t="inlineStr">
         <is>
           <t>Serving Trays</t>
         </is>
@@ -1382,7 +1282,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1434,25 +1334,21 @@
     </row>
     <row r="2">
       <c r="A2" s="8" t="n">
-        <v>44309.62232832416</v>
+        <v>44309.69305795074</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
           <t>B08R3HNBMF</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>CHECKED EMPTY</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>CHECKED EMPTY</t>
-        </is>
+      <c r="C2" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="D2" t="n">
+        <v>2</v>
       </c>
       <c r="E2" t="n">
-        <v>64835</v>
+        <v>72726</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -1460,105 +1356,9 @@
         </is>
       </c>
       <c r="G2" t="n">
-        <v>453</v>
+        <v>518</v>
       </c>
       <c r="H2" t="inlineStr">
-        <is>
-          <t>Serving Trays</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="8" t="n">
-        <v>44309.6236936315</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>B08R3HNBMF</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="D3" t="n">
-        <v>2</v>
-      </c>
-      <c r="E3" t="n">
-        <v>72726</v>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Kitchen &amp; Dining</t>
-        </is>
-      </c>
-      <c r="G3" t="n">
-        <v>518</v>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>Serving Trays</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="8" t="n">
-        <v>44309.62842238994</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>B08R3HNBMF</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="D4" t="n">
-        <v>2</v>
-      </c>
-      <c r="E4" t="n">
-        <v>72726</v>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Kitchen &amp; Dining</t>
-        </is>
-      </c>
-      <c r="G4" t="n">
-        <v>518</v>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>Serving Trays</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="8" t="n">
-        <v>44309.63155193812</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>B08R3HNBMF</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="D5" t="n">
-        <v>2</v>
-      </c>
-      <c r="E5" t="n">
-        <v>72726</v>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>Kitchen &amp; Dining</t>
-        </is>
-      </c>
-      <c r="G5" t="n">
-        <v>518</v>
-      </c>
-      <c r="H5" t="inlineStr">
         <is>
           <t>Serving Trays</t>
         </is>
@@ -1575,7 +1375,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1627,25 +1427,21 @@
     </row>
     <row r="2">
       <c r="A2" s="8" t="n">
-        <v>44309.62235229951</v>
+        <v>44309.69308349252</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
           <t>B08R3HH8P8</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>CHECKED EMPTY</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>CHECKED EMPTY</t>
-        </is>
+      <c r="C2" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="D2" t="n">
+        <v>2</v>
       </c>
       <c r="E2" t="n">
-        <v>64835</v>
+        <v>72726</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -1653,105 +1449,9 @@
         </is>
       </c>
       <c r="G2" t="n">
-        <v>453</v>
+        <v>518</v>
       </c>
       <c r="H2" t="inlineStr">
-        <is>
-          <t>Serving Trays</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="8" t="n">
-        <v>44309.62371298977</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>B08R3HH8P8</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="D3" t="n">
-        <v>2</v>
-      </c>
-      <c r="E3" t="n">
-        <v>72726</v>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Kitchen &amp; Dining</t>
-        </is>
-      </c>
-      <c r="G3" t="n">
-        <v>518</v>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>Serving Trays</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="8" t="n">
-        <v>44309.62844563591</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>B08R3HH8P8</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="D4" t="n">
-        <v>2</v>
-      </c>
-      <c r="E4" t="n">
-        <v>72726</v>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Kitchen &amp; Dining</t>
-        </is>
-      </c>
-      <c r="G4" t="n">
-        <v>518</v>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>Serving Trays</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="8" t="n">
-        <v>44309.63157389128</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>B08R3HH8P8</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="D5" t="n">
-        <v>2</v>
-      </c>
-      <c r="E5" t="n">
-        <v>72726</v>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>Kitchen &amp; Dining</t>
-        </is>
-      </c>
-      <c r="G5" t="n">
-        <v>518</v>
-      </c>
-      <c r="H5" t="inlineStr">
         <is>
           <t>Serving Trays</t>
         </is>
@@ -1768,7 +1468,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1820,25 +1520,21 @@
     </row>
     <row r="2">
       <c r="A2" s="8" t="n">
-        <v>44309.62237056768</v>
+        <v>44309.6931038873</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
           <t>B088RB1GRD</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>CHECKED EMPTY</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>CHECKED EMPTY</t>
-        </is>
+      <c r="C2" t="n">
+        <v>4.4</v>
+      </c>
+      <c r="D2" t="n">
+        <v>169</v>
       </c>
       <c r="E2" t="n">
-        <v>70260</v>
+        <v>81452</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -1846,105 +1542,9 @@
         </is>
       </c>
       <c r="G2" t="n">
-        <v>86</v>
+        <v>106</v>
       </c>
       <c r="H2" t="inlineStr">
-        <is>
-          <t>Decorative Boxes</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="8" t="n">
-        <v>44309.62373815116</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>B088RB1GRD</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>4.4</v>
-      </c>
-      <c r="D3" t="n">
-        <v>169</v>
-      </c>
-      <c r="E3" t="n">
-        <v>81452</v>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Home &amp; Kitchen</t>
-        </is>
-      </c>
-      <c r="G3" t="n">
-        <v>106</v>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>Decorative Boxes</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="8" t="n">
-        <v>44309.62846267061</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>B088RB1GRD</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>4.4</v>
-      </c>
-      <c r="D4" t="n">
-        <v>169</v>
-      </c>
-      <c r="E4" t="n">
-        <v>81452</v>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Home &amp; Kitchen</t>
-        </is>
-      </c>
-      <c r="G4" t="n">
-        <v>106</v>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>Decorative Boxes</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="8" t="n">
-        <v>44309.63159317279</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>B088RB1GRD</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>4.4</v>
-      </c>
-      <c r="D5" t="n">
-        <v>169</v>
-      </c>
-      <c r="E5" t="n">
-        <v>81452</v>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>Home &amp; Kitchen</t>
-        </is>
-      </c>
-      <c r="G5" t="n">
-        <v>106</v>
-      </c>
-      <c r="H5" t="inlineStr">
         <is>
           <t>Decorative Boxes</t>
         </is>
@@ -1961,7 +1561,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2013,25 +1613,21 @@
     </row>
     <row r="2">
       <c r="A2" s="8" t="n">
-        <v>44309.62239305667</v>
+        <v>44309.69312686843</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
           <t>B08R3LN8NH</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>CHECKED EMPTY</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>CHECKED EMPTY</t>
-        </is>
+      <c r="C2" t="n">
+        <v>4.3</v>
+      </c>
+      <c r="D2" t="n">
+        <v>11</v>
       </c>
       <c r="E2" t="n">
-        <v>185361</v>
+        <v>166014</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -2039,105 +1635,9 @@
         </is>
       </c>
       <c r="G2" t="n">
-        <v>724</v>
+        <v>683</v>
       </c>
       <c r="H2" t="inlineStr">
-        <is>
-          <t>Floating Shelves</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="8" t="n">
-        <v>44309.62375638798</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>B08R3LN8NH</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>4.3</v>
-      </c>
-      <c r="D3" t="n">
-        <v>11</v>
-      </c>
-      <c r="E3" t="n">
-        <v>185361</v>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Home &amp; Kitchen</t>
-        </is>
-      </c>
-      <c r="G3" t="n">
-        <v>724</v>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>Floating Shelves</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="8" t="n">
-        <v>44309.62848946742</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>B08R3LN8NH</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>4.3</v>
-      </c>
-      <c r="D4" t="n">
-        <v>11</v>
-      </c>
-      <c r="E4" t="n">
-        <v>185361</v>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Home &amp; Kitchen</t>
-        </is>
-      </c>
-      <c r="G4" t="n">
-        <v>724</v>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>Floating Shelves</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="8" t="n">
-        <v>44309.63161551388</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>B08R3LN8NH</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>4.3</v>
-      </c>
-      <c r="D5" t="n">
-        <v>11</v>
-      </c>
-      <c r="E5" t="n">
-        <v>185361</v>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>Home &amp; Kitchen</t>
-        </is>
-      </c>
-      <c r="G5" t="n">
-        <v>724</v>
-      </c>
-      <c r="H5" t="inlineStr">
         <is>
           <t>Floating Shelves</t>
         </is>
@@ -2154,7 +1654,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2206,7 +1706,7 @@
     </row>
     <row r="2">
       <c r="A2" s="8" t="n">
-        <v>44309.63163404034</v>
+        <v>44309.69315105717</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -2239,86 +1739,6 @@
         </is>
       </c>
       <c r="H2" t="inlineStr">
-        <is>
-          <t>NAN</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="8" t="n">
-        <v>44309.63163670638</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>NAN</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>NAN</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>NAN</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>NAN</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>NAN</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>NAN</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="8" t="n">
-        <v>44309.63163938937</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>NAN</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>NAN</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>NAN</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>NAN</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>NAN</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
         <is>
           <t>NAN</t>
         </is>
@@ -2335,7 +1755,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2382,6 +1802,46 @@
       <c r="H1" t="inlineStr">
         <is>
           <t>RANKING2_CAT</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="8" t="n">
+        <v>44309.69315424914</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>NAN</t>
         </is>
       </c>
     </row>
@@ -2396,7 +1856,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2443,6 +1903,46 @@
       <c r="H1" t="inlineStr">
         <is>
           <t>RANKING2_CAT</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="8" t="n">
+        <v>44309.69315731672</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>NAN</t>
         </is>
       </c>
     </row>
@@ -2457,7 +1957,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2509,25 +2009,21 @@
     </row>
     <row r="2">
       <c r="A2" s="8" t="n">
-        <v>44309.62242224805</v>
+        <v>44309.69316040542</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
           <t>B087D7VP7B</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>CHECKED EMPTY</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>CHECKED EMPTY</t>
-        </is>
+      <c r="C2" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="D2" t="n">
+        <v>163</v>
       </c>
       <c r="E2" t="n">
-        <v>182335</v>
+        <v>206436</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -2535,105 +2031,9 @@
         </is>
       </c>
       <c r="G2" t="n">
-        <v>134</v>
+        <v>149</v>
       </c>
       <c r="H2" t="inlineStr">
-        <is>
-          <t>Decorative Trays</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="8" t="n">
-        <v>44309.62378769556</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>B087D7VP7B</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>4.6</v>
-      </c>
-      <c r="D3" t="n">
-        <v>163</v>
-      </c>
-      <c r="E3" t="n">
-        <v>182335</v>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Home &amp; Kitchen</t>
-        </is>
-      </c>
-      <c r="G3" t="n">
-        <v>134</v>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>Decorative Trays</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="8" t="n">
-        <v>44309.62851886986</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>B087D7VP7B</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>4.6</v>
-      </c>
-      <c r="D4" t="n">
-        <v>163</v>
-      </c>
-      <c r="E4" t="n">
-        <v>206436</v>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Home &amp; Kitchen</t>
-        </is>
-      </c>
-      <c r="G4" t="n">
-        <v>149</v>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>Decorative Trays</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="8" t="n">
-        <v>44309.63164210684</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>B087D7VP7B</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>4.6</v>
-      </c>
-      <c r="D5" t="n">
-        <v>163</v>
-      </c>
-      <c r="E5" t="n">
-        <v>206436</v>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>Home &amp; Kitchen</t>
-        </is>
-      </c>
-      <c r="G5" t="n">
-        <v>149</v>
-      </c>
-      <c r="H5" t="inlineStr">
         <is>
           <t>Decorative Trays</t>
         </is>
@@ -2650,7 +2050,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2702,25 +2102,21 @@
     </row>
     <row r="2">
       <c r="A2" s="8" t="n">
-        <v>44309.62244347918</v>
+        <v>44309.69318463845</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
           <t>B087D7VP7B</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>CHECKED EMPTY</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>CHECKED EMPTY</t>
-        </is>
+      <c r="C2" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="D2" t="n">
+        <v>163</v>
       </c>
       <c r="E2" t="n">
-        <v>182335</v>
+        <v>206436</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -2728,105 +2124,9 @@
         </is>
       </c>
       <c r="G2" t="n">
-        <v>134</v>
+        <v>149</v>
       </c>
       <c r="H2" t="inlineStr">
-        <is>
-          <t>Decorative Trays</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="8" t="n">
-        <v>44309.62381118967</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>B087D7VP7B</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>4.6</v>
-      </c>
-      <c r="D3" t="n">
-        <v>163</v>
-      </c>
-      <c r="E3" t="n">
-        <v>182335</v>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Home &amp; Kitchen</t>
-        </is>
-      </c>
-      <c r="G3" t="n">
-        <v>134</v>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>Decorative Trays</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="8" t="n">
-        <v>44309.62854175881</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>B087D7VP7B</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>4.6</v>
-      </c>
-      <c r="D4" t="n">
-        <v>163</v>
-      </c>
-      <c r="E4" t="n">
-        <v>206436</v>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Home &amp; Kitchen</t>
-        </is>
-      </c>
-      <c r="G4" t="n">
-        <v>149</v>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>Decorative Trays</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="8" t="n">
-        <v>44309.63166388765</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>B087D7VP7B</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>4.6</v>
-      </c>
-      <c r="D5" t="n">
-        <v>163</v>
-      </c>
-      <c r="E5" t="n">
-        <v>206436</v>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>Home &amp; Kitchen</t>
-        </is>
-      </c>
-      <c r="G5" t="n">
-        <v>149</v>
-      </c>
-      <c r="H5" t="inlineStr">
         <is>
           <t>Decorative Trays</t>
         </is>
@@ -2843,7 +2143,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2895,22 +2195,18 @@
     </row>
     <row r="2">
       <c r="A2" s="8" t="n">
-        <v>44309.62213960902</v>
+        <v>44309.6928730228</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
           <t>B07F6YFT4F</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>CHECKED EMPTY</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>CHECKED EMPTY</t>
-        </is>
+      <c r="C2" t="n">
+        <v>4.4</v>
+      </c>
+      <c r="D2" t="n">
+        <v>1650</v>
       </c>
       <c r="E2" t="n">
         <v>68308</v>
@@ -2924,102 +2220,6 @@
         <v>284</v>
       </c>
       <c r="H2" t="inlineStr">
-        <is>
-          <t>Indoor String Lights</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="8" t="n">
-        <v>44309.62348518416</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>B07F6YFT4F</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>4.4</v>
-      </c>
-      <c r="D3" t="n">
-        <v>1649</v>
-      </c>
-      <c r="E3" t="n">
-        <v>68308</v>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Home &amp; Kitchen</t>
-        </is>
-      </c>
-      <c r="G3" t="n">
-        <v>284</v>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>Indoor String Lights</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="8" t="n">
-        <v>44309.62825413198</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>B07F6YFT4F</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>4.4</v>
-      </c>
-      <c r="D4" t="n">
-        <v>1649</v>
-      </c>
-      <c r="E4" t="n">
-        <v>68308</v>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Home &amp; Kitchen</t>
-        </is>
-      </c>
-      <c r="G4" t="n">
-        <v>284</v>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>Indoor String Lights</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="8" t="n">
-        <v>44309.63136690284</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>B07F6YFT4F</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>4.4</v>
-      </c>
-      <c r="D5" t="n">
-        <v>1649</v>
-      </c>
-      <c r="E5" t="n">
-        <v>68308</v>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>Home &amp; Kitchen</t>
-        </is>
-      </c>
-      <c r="G5" t="n">
-        <v>284</v>
-      </c>
-      <c r="H5" t="inlineStr">
         <is>
           <t>Indoor String Lights</t>
         </is>
@@ -3036,7 +2236,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3088,25 +2288,21 @@
     </row>
     <row r="2">
       <c r="A2" s="8" t="n">
-        <v>44309.62246394109</v>
+        <v>44309.69320218355</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
           <t>B088RDY8YS</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>CHECKED EMPTY</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>CHECKED EMPTY</t>
-        </is>
+      <c r="C2" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="D2" t="n">
+        <v>127</v>
       </c>
       <c r="E2" t="n">
-        <v>173623</v>
+        <v>196384</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -3114,105 +2310,9 @@
         </is>
       </c>
       <c r="G2" t="n">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="H2" t="inlineStr">
-        <is>
-          <t>Sculptural Picture Frames &amp; Holders</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="8" t="n">
-        <v>44309.62382980756</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>B088RDY8YS</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="D3" t="n">
-        <v>127</v>
-      </c>
-      <c r="E3" t="n">
-        <v>173623</v>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Home &amp; Kitchen</t>
-        </is>
-      </c>
-      <c r="G3" t="n">
-        <v>22</v>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>Sculptural Picture Frames &amp; Holders</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="8" t="n">
-        <v>44309.62855982583</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>B088RDY8YS</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="D4" t="n">
-        <v>127</v>
-      </c>
-      <c r="E4" t="n">
-        <v>173623</v>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Home &amp; Kitchen</t>
-        </is>
-      </c>
-      <c r="G4" t="n">
-        <v>22</v>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>Sculptural Picture Frames &amp; Holders</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="8" t="n">
-        <v>44309.6316815336</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>B088RDY8YS</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="D5" t="n">
-        <v>127</v>
-      </c>
-      <c r="E5" t="n">
-        <v>173623</v>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>Home &amp; Kitchen</t>
-        </is>
-      </c>
-      <c r="G5" t="n">
-        <v>22</v>
-      </c>
-      <c r="H5" t="inlineStr">
         <is>
           <t>Sculptural Picture Frames &amp; Holders</t>
         </is>
@@ -3229,7 +2329,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3281,25 +2381,21 @@
     </row>
     <row r="2">
       <c r="A2" s="8" t="n">
-        <v>44309.62248348516</v>
+        <v>44309.69322519479</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
           <t>B088RD9XK6</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>CHECKED EMPTY</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>CHECKED EMPTY</t>
-        </is>
+      <c r="C2" t="n">
+        <v>4.7</v>
+      </c>
+      <c r="D2" t="n">
+        <v>58</v>
       </c>
       <c r="E2" t="n">
-        <v>71421</v>
+        <v>83260</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -3307,105 +2403,9 @@
         </is>
       </c>
       <c r="G2" t="n">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="H2" t="inlineStr">
-        <is>
-          <t>Decorative Bookends</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="8" t="n">
-        <v>44309.62384922076</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>B088RD9XK6</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>4.7</v>
-      </c>
-      <c r="D3" t="n">
-        <v>58</v>
-      </c>
-      <c r="E3" t="n">
-        <v>83260</v>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Home &amp; Kitchen</t>
-        </is>
-      </c>
-      <c r="G3" t="n">
-        <v>16</v>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>Decorative Bookends</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="8" t="n">
-        <v>44309.62858126473</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>B088RD9XK6</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>4.7</v>
-      </c>
-      <c r="D4" t="n">
-        <v>58</v>
-      </c>
-      <c r="E4" t="n">
-        <v>83260</v>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Home &amp; Kitchen</t>
-        </is>
-      </c>
-      <c r="G4" t="n">
-        <v>16</v>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>Decorative Bookends</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="8" t="n">
-        <v>44309.63170057337</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>B088RD9XK6</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>4.7</v>
-      </c>
-      <c r="D5" t="n">
-        <v>58</v>
-      </c>
-      <c r="E5" t="n">
-        <v>83260</v>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>Home &amp; Kitchen</t>
-        </is>
-      </c>
-      <c r="G5" t="n">
-        <v>16</v>
-      </c>
-      <c r="H5" t="inlineStr">
         <is>
           <t>Decorative Bookends</t>
         </is>
@@ -3422,7 +2422,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3474,22 +2474,18 @@
     </row>
     <row r="2">
       <c r="A2" s="8" t="n">
-        <v>44309.62250704824</v>
+        <v>44309.69324976933</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
           <t>B088RC9TNP</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>CHECKED EMPTY</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>CHECKED EMPTY</t>
-        </is>
+      <c r="C2" t="n">
+        <v>4.7</v>
+      </c>
+      <c r="D2" t="n">
+        <v>58</v>
       </c>
       <c r="E2" t="n">
         <v>83260</v>
@@ -3503,102 +2499,6 @@
         <v>16</v>
       </c>
       <c r="H2" t="inlineStr">
-        <is>
-          <t>Decorative Bookends</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="8" t="n">
-        <v>44309.62386948505</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>B088RC9TNP</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>4.7</v>
-      </c>
-      <c r="D3" t="n">
-        <v>58</v>
-      </c>
-      <c r="E3" t="n">
-        <v>83260</v>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Home &amp; Kitchen</t>
-        </is>
-      </c>
-      <c r="G3" t="n">
-        <v>16</v>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>Decorative Bookends</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="8" t="n">
-        <v>44309.62860353741</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>B088RC9TNP</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>4.7</v>
-      </c>
-      <c r="D4" t="n">
-        <v>58</v>
-      </c>
-      <c r="E4" t="n">
-        <v>83260</v>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Home &amp; Kitchen</t>
-        </is>
-      </c>
-      <c r="G4" t="n">
-        <v>16</v>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>Decorative Bookends</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="8" t="n">
-        <v>44309.63172175697</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>B088RC9TNP</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>4.7</v>
-      </c>
-      <c r="D5" t="n">
-        <v>58</v>
-      </c>
-      <c r="E5" t="n">
-        <v>83260</v>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>Home &amp; Kitchen</t>
-        </is>
-      </c>
-      <c r="G5" t="n">
-        <v>16</v>
-      </c>
-      <c r="H5" t="inlineStr">
         <is>
           <t>Decorative Bookends</t>
         </is>
@@ -3615,7 +2515,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3667,22 +2567,18 @@
     </row>
     <row r="2">
       <c r="A2" s="8" t="n">
-        <v>44309.62252855993</v>
+        <v>44309.69327036794</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
           <t>B088RD9XK6</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>CHECKED EMPTY</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>CHECKED EMPTY</t>
-        </is>
+      <c r="C2" t="n">
+        <v>4.7</v>
+      </c>
+      <c r="D2" t="n">
+        <v>58</v>
       </c>
       <c r="E2" t="n">
         <v>83260</v>
@@ -3696,102 +2592,6 @@
         <v>16</v>
       </c>
       <c r="H2" t="inlineStr">
-        <is>
-          <t>Decorative Bookends</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="8" t="n">
-        <v>44309.62388934792</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>B088RD9XK6</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>4.7</v>
-      </c>
-      <c r="D3" t="n">
-        <v>58</v>
-      </c>
-      <c r="E3" t="n">
-        <v>83260</v>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Home &amp; Kitchen</t>
-        </is>
-      </c>
-      <c r="G3" t="n">
-        <v>16</v>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>Decorative Bookends</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="8" t="n">
-        <v>44309.62862363507</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>B088RD9XK6</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>4.7</v>
-      </c>
-      <c r="D4" t="n">
-        <v>58</v>
-      </c>
-      <c r="E4" t="n">
-        <v>83260</v>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Home &amp; Kitchen</t>
-        </is>
-      </c>
-      <c r="G4" t="n">
-        <v>16</v>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>Decorative Bookends</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="8" t="n">
-        <v>44309.63174223751</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>B088RD9XK6</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>4.7</v>
-      </c>
-      <c r="D5" t="n">
-        <v>58</v>
-      </c>
-      <c r="E5" t="n">
-        <v>83260</v>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>Home &amp; Kitchen</t>
-        </is>
-      </c>
-      <c r="G5" t="n">
-        <v>16</v>
-      </c>
-      <c r="H5" t="inlineStr">
         <is>
           <t>Decorative Bookends</t>
         </is>
@@ -3860,7 +2660,7 @@
     </row>
     <row r="2">
       <c r="A2" s="8" t="n">
-        <v>44309.63176156989</v>
+        <v>44309.69329471978</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -3961,7 +2761,7 @@
     </row>
     <row r="2">
       <c r="A2" s="8" t="n">
-        <v>44309.63177476068</v>
+        <v>44309.69330698111</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -4062,7 +2862,7 @@
     </row>
     <row r="2">
       <c r="A2" s="8" t="n">
-        <v>44309.63178774781</v>
+        <v>44309.69331913685</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -4111,7 +2911,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4163,25 +2963,21 @@
     </row>
     <row r="2">
       <c r="A2" s="8" t="n">
-        <v>44309.62259752223</v>
+        <v>44309.69333142805</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
           <t>B08RDDR92G</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>CHECKED EMPTY</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>CHECKED EMPTY</t>
-        </is>
+      <c r="C2" t="n">
+        <v>3.8</v>
+      </c>
+      <c r="D2" t="n">
+        <v>9</v>
       </c>
       <c r="E2" t="n">
-        <v>59042</v>
+        <v>63280</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -4189,105 +2985,9 @@
         </is>
       </c>
       <c r="G2" t="n">
-        <v>327</v>
+        <v>352</v>
       </c>
       <c r="H2" t="inlineStr">
-        <is>
-          <t>Artificial Plants &amp; Greenery</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="8" t="n">
-        <v>44309.62395488589</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>B08RDDR92G</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>3.8</v>
-      </c>
-      <c r="D3" t="n">
-        <v>9</v>
-      </c>
-      <c r="E3" t="n">
-        <v>59042</v>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Home &amp; Kitchen</t>
-        </is>
-      </c>
-      <c r="G3" t="n">
-        <v>327</v>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>Artificial Plants &amp; Greenery</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="8" t="n">
-        <v>44309.62869862317</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>B08RDDR92G</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>3.8</v>
-      </c>
-      <c r="D4" t="n">
-        <v>9</v>
-      </c>
-      <c r="E4" t="n">
-        <v>59042</v>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Home &amp; Kitchen</t>
-        </is>
-      </c>
-      <c r="G4" t="n">
-        <v>327</v>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>Artificial Plants &amp; Greenery</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="8" t="n">
-        <v>44309.63180279901</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>B08RDDR92G</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>3.8</v>
-      </c>
-      <c r="D5" t="n">
-        <v>9</v>
-      </c>
-      <c r="E5" t="n">
-        <v>59042</v>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>Home &amp; Kitchen</t>
-        </is>
-      </c>
-      <c r="G5" t="n">
-        <v>327</v>
-      </c>
-      <c r="H5" t="inlineStr">
         <is>
           <t>Artificial Plants &amp; Greenery</t>
         </is>
@@ -4304,7 +3004,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4356,22 +3056,18 @@
     </row>
     <row r="2">
       <c r="A2" s="8" t="n">
-        <v>44309.62261755508</v>
+        <v>44309.69335371384</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
           <t>B08RDCBV6V</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>CHECKED EMPTY</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>CHECKED EMPTY</t>
-        </is>
+      <c r="C2" t="n">
+        <v>3.8</v>
+      </c>
+      <c r="D2" t="n">
+        <v>9</v>
       </c>
       <c r="E2" t="n">
         <v>63280</v>
@@ -4385,102 +3081,6 @@
         <v>352</v>
       </c>
       <c r="H2" t="inlineStr">
-        <is>
-          <t>Artificial Plants &amp; Greenery</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="8" t="n">
-        <v>44309.6239766817</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>B08RDCBV6V</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>3.8</v>
-      </c>
-      <c r="D3" t="n">
-        <v>9</v>
-      </c>
-      <c r="E3" t="n">
-        <v>63280</v>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Home &amp; Kitchen</t>
-        </is>
-      </c>
-      <c r="G3" t="n">
-        <v>352</v>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>Artificial Plants &amp; Greenery</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="8" t="n">
-        <v>44309.62872312323</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>B08RDCBV6V</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>3.8</v>
-      </c>
-      <c r="D4" t="n">
-        <v>9</v>
-      </c>
-      <c r="E4" t="n">
-        <v>63280</v>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Home &amp; Kitchen</t>
-        </is>
-      </c>
-      <c r="G4" t="n">
-        <v>352</v>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>Artificial Plants &amp; Greenery</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="8" t="n">
-        <v>44309.6318252784</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>B08RDCBV6V</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>3.8</v>
-      </c>
-      <c r="D5" t="n">
-        <v>9</v>
-      </c>
-      <c r="E5" t="n">
-        <v>63280</v>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>Home &amp; Kitchen</t>
-        </is>
-      </c>
-      <c r="G5" t="n">
-        <v>352</v>
-      </c>
-      <c r="H5" t="inlineStr">
         <is>
           <t>Artificial Plants &amp; Greenery</t>
         </is>
@@ -4497,7 +3097,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4549,25 +3149,21 @@
     </row>
     <row r="2">
       <c r="A2" s="8" t="n">
-        <v>44309.62263630877</v>
+        <v>44309.69337152607</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
           <t>B08RJ7S3Y5</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>CHECKED EMPTY</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>CHECKED EMPTY</t>
-        </is>
+      <c r="C2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D2" t="n">
+        <v>6</v>
       </c>
       <c r="E2" t="n">
-        <v>112638</v>
+        <v>130805</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -4575,105 +3171,9 @@
         </is>
       </c>
       <c r="G2" t="n">
-        <v>1185</v>
+        <v>1413</v>
       </c>
       <c r="H2" t="inlineStr">
-        <is>
-          <t>Artificial Flowers</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="8" t="n">
-        <v>44309.62399698015</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>B08RJ7S3Y5</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>2</v>
-      </c>
-      <c r="D3" t="n">
-        <v>6</v>
-      </c>
-      <c r="E3" t="n">
-        <v>112638</v>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Home &amp; Kitchen</t>
-        </is>
-      </c>
-      <c r="G3" t="n">
-        <v>1185</v>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>Artificial Flowers</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="8" t="n">
-        <v>44309.62874134369</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>B08RJ7S3Y5</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>2</v>
-      </c>
-      <c r="D4" t="n">
-        <v>6</v>
-      </c>
-      <c r="E4" t="n">
-        <v>130805</v>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Home &amp; Kitchen</t>
-        </is>
-      </c>
-      <c r="G4" t="n">
-        <v>1413</v>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>Artificial Flowers</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="8" t="n">
-        <v>44309.6318420356</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>B08RJ7S3Y5</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>2</v>
-      </c>
-      <c r="D5" t="n">
-        <v>6</v>
-      </c>
-      <c r="E5" t="n">
-        <v>130805</v>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>Home &amp; Kitchen</t>
-        </is>
-      </c>
-      <c r="G5" t="n">
-        <v>1413</v>
-      </c>
-      <c r="H5" t="inlineStr">
         <is>
           <t>Artificial Flowers</t>
         </is>
@@ -4690,7 +3190,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4742,22 +3242,18 @@
     </row>
     <row r="2">
       <c r="A2" s="8" t="n">
-        <v>44309.62216383131</v>
+        <v>44309.69290122313</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
           <t>B07F1FWK43</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>CHECKED EMPTY</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>CHECKED EMPTY</t>
-        </is>
+      <c r="C2" t="n">
+        <v>4.4</v>
+      </c>
+      <c r="D2" t="n">
+        <v>1650</v>
       </c>
       <c r="E2" t="n">
         <v>68308</v>
@@ -4771,102 +3267,6 @@
         <v>284</v>
       </c>
       <c r="H2" t="inlineStr">
-        <is>
-          <t>Indoor String Lights</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="8" t="n">
-        <v>44309.62350842408</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>B07F1FWK43</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>4.4</v>
-      </c>
-      <c r="D3" t="n">
-        <v>1649</v>
-      </c>
-      <c r="E3" t="n">
-        <v>68308</v>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Home &amp; Kitchen</t>
-        </is>
-      </c>
-      <c r="G3" t="n">
-        <v>284</v>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>Indoor String Lights</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="8" t="n">
-        <v>44309.62827498929</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>B07F1FWK43</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>4.4</v>
-      </c>
-      <c r="D4" t="n">
-        <v>1649</v>
-      </c>
-      <c r="E4" t="n">
-        <v>68308</v>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Home &amp; Kitchen</t>
-        </is>
-      </c>
-      <c r="G4" t="n">
-        <v>284</v>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>Indoor String Lights</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="8" t="n">
-        <v>44309.63139027423</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>B07F1FWK43</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>4.4</v>
-      </c>
-      <c r="D5" t="n">
-        <v>1649</v>
-      </c>
-      <c r="E5" t="n">
-        <v>68308</v>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>Home &amp; Kitchen</t>
-        </is>
-      </c>
-      <c r="G5" t="n">
-        <v>284</v>
-      </c>
-      <c r="H5" t="inlineStr">
         <is>
           <t>Indoor String Lights</t>
         </is>
@@ -4883,7 +3283,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4935,22 +3335,18 @@
     </row>
     <row r="2">
       <c r="A2" s="8" t="n">
-        <v>44309.62266426567</v>
+        <v>44309.69339237434</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
           <t>B08RJG6YMP</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>CHECKED EMPTY</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>CHECKED EMPTY</t>
-        </is>
+      <c r="C2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D2" t="n">
+        <v>6</v>
       </c>
       <c r="E2" t="n">
         <v>130805</v>
@@ -4964,102 +3360,6 @@
         <v>1413</v>
       </c>
       <c r="H2" t="inlineStr">
-        <is>
-          <t>Artificial Flowers</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="8" t="n">
-        <v>44309.62401746141</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>B08RJG6YMP</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>2</v>
-      </c>
-      <c r="D3" t="n">
-        <v>6</v>
-      </c>
-      <c r="E3" t="n">
-        <v>130805</v>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Home &amp; Kitchen</t>
-        </is>
-      </c>
-      <c r="G3" t="n">
-        <v>1413</v>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>Artificial Flowers</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="8" t="n">
-        <v>44309.62876165493</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>B08RJG6YMP</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>2</v>
-      </c>
-      <c r="D4" t="n">
-        <v>6</v>
-      </c>
-      <c r="E4" t="n">
-        <v>130805</v>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Home &amp; Kitchen</t>
-        </is>
-      </c>
-      <c r="G4" t="n">
-        <v>1413</v>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>Artificial Flowers</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="8" t="n">
-        <v>44309.6318616443</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>B08RJG6YMP</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>2</v>
-      </c>
-      <c r="D5" t="n">
-        <v>6</v>
-      </c>
-      <c r="E5" t="n">
-        <v>130805</v>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>Home &amp; Kitchen</t>
-        </is>
-      </c>
-      <c r="G5" t="n">
-        <v>1413</v>
-      </c>
-      <c r="H5" t="inlineStr">
         <is>
           <t>Artificial Flowers</t>
         </is>
@@ -5076,7 +3376,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5128,7 +3428,7 @@
     </row>
     <row r="2">
       <c r="A2" s="8" t="n">
-        <v>44309.62268211621</v>
+        <v>44309.69341404419</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -5146,7 +3446,7 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>129086</v>
+        <v>152958</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -5154,117 +3454,9 @@
         </is>
       </c>
       <c r="G2" t="n">
-        <v>298</v>
+        <v>363</v>
       </c>
       <c r="H2" t="inlineStr">
-        <is>
-          <t>Jewelry Trays</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="8" t="n">
-        <v>44309.62403998911</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>B08RYPRTTF</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>CHECKED EMPTY</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>CHECKED EMPTY</t>
-        </is>
-      </c>
-      <c r="E3" t="n">
-        <v>129086</v>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Clothing, Shoes &amp; Jewelry</t>
-        </is>
-      </c>
-      <c r="G3" t="n">
-        <v>298</v>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>Jewelry Trays</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="8" t="n">
-        <v>44309.62878003084</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>B08RYPRTTF</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>CHECKED EMPTY</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>CHECKED EMPTY</t>
-        </is>
-      </c>
-      <c r="E4" t="n">
-        <v>129086</v>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Clothing, Shoes &amp; Jewelry</t>
-        </is>
-      </c>
-      <c r="G4" t="n">
-        <v>298</v>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>Jewelry Trays</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="8" t="n">
-        <v>44309.63188043156</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>B08RYPRTTF</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>CHECKED EMPTY</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>CHECKED EMPTY</t>
-        </is>
-      </c>
-      <c r="E5" t="n">
-        <v>152958</v>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>Clothing, Shoes &amp; Jewelry</t>
-        </is>
-      </c>
-      <c r="G5" t="n">
-        <v>363</v>
-      </c>
-      <c r="H5" t="inlineStr">
         <is>
           <t>Jewelry Trays</t>
         </is>
@@ -5281,7 +3473,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5333,7 +3525,7 @@
     </row>
     <row r="2">
       <c r="A2" s="8" t="n">
-        <v>44309.62270508092</v>
+        <v>44309.69343968834</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -5362,114 +3554,6 @@
         <v>363</v>
       </c>
       <c r="H2" t="inlineStr">
-        <is>
-          <t>Jewelry Trays</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="8" t="n">
-        <v>44309.62406018686</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>B08RYQX56M</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>CHECKED EMPTY</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>CHECKED EMPTY</t>
-        </is>
-      </c>
-      <c r="E3" t="n">
-        <v>152958</v>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Clothing, Shoes &amp; Jewelry</t>
-        </is>
-      </c>
-      <c r="G3" t="n">
-        <v>363</v>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>Jewelry Trays</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="8" t="n">
-        <v>44309.62881645439</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>B08RYQX56M</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>CHECKED EMPTY</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>CHECKED EMPTY</t>
-        </is>
-      </c>
-      <c r="E4" t="n">
-        <v>152958</v>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Clothing, Shoes &amp; Jewelry</t>
-        </is>
-      </c>
-      <c r="G4" t="n">
-        <v>363</v>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>Jewelry Trays</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="8" t="n">
-        <v>44309.63190602948</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>B08RYQX56M</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>CHECKED EMPTY</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>CHECKED EMPTY</t>
-        </is>
-      </c>
-      <c r="E5" t="n">
-        <v>152958</v>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>Clothing, Shoes &amp; Jewelry</t>
-        </is>
-      </c>
-      <c r="G5" t="n">
-        <v>363</v>
-      </c>
-      <c r="H5" t="inlineStr">
         <is>
           <t>Jewelry Trays</t>
         </is>
@@ -5486,7 +3570,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5538,22 +3622,18 @@
     </row>
     <row r="2">
       <c r="A2" s="8" t="n">
-        <v>44309.62273552818</v>
+        <v>44309.69346341551</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
           <t>B08RYN4M1J</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>CHECKED EMPTY</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>CHECKED EMPTY</t>
-        </is>
+      <c r="C2" t="n">
+        <v>5</v>
+      </c>
+      <c r="D2" t="n">
+        <v>3</v>
       </c>
       <c r="E2" t="n">
         <v>122059</v>
@@ -5567,102 +3647,6 @@
         <v>282</v>
       </c>
       <c r="H2" t="inlineStr">
-        <is>
-          <t>Jewelry Trays</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="8" t="n">
-        <v>44309.62407920212</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>B08RYN4M1J</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>5</v>
-      </c>
-      <c r="D3" t="n">
-        <v>3</v>
-      </c>
-      <c r="E3" t="n">
-        <v>122059</v>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Clothing, Shoes &amp; Jewelry</t>
-        </is>
-      </c>
-      <c r="G3" t="n">
-        <v>282</v>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>Jewelry Trays</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="8" t="n">
-        <v>44309.62883529333</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>B08RYN4M1J</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>5</v>
-      </c>
-      <c r="D4" t="n">
-        <v>3</v>
-      </c>
-      <c r="E4" t="n">
-        <v>122059</v>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Clothing, Shoes &amp; Jewelry</t>
-        </is>
-      </c>
-      <c r="G4" t="n">
-        <v>282</v>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>Jewelry Trays</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="8" t="n">
-        <v>44309.63192599613</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>B08RYN4M1J</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>5</v>
-      </c>
-      <c r="D5" t="n">
-        <v>3</v>
-      </c>
-      <c r="E5" t="n">
-        <v>122059</v>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>Clothing, Shoes &amp; Jewelry</t>
-        </is>
-      </c>
-      <c r="G5" t="n">
-        <v>282</v>
-      </c>
-      <c r="H5" t="inlineStr">
         <is>
           <t>Jewelry Trays</t>
         </is>
@@ -5679,7 +3663,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5731,7 +3715,7 @@
     </row>
     <row r="2">
       <c r="A2" s="8" t="n">
-        <v>44309.62275438791</v>
+        <v>44309.69349871631</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -5749,7 +3733,7 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>259538</v>
+        <v>307550</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -5757,117 +3741,9 @@
         </is>
       </c>
       <c r="G2" t="n">
-        <v>635</v>
+        <v>745</v>
       </c>
       <c r="H2" t="inlineStr">
-        <is>
-          <t>Jewelry Trays</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="8" t="n">
-        <v>44309.62409803915</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>B08RYQ3JKD</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>CHECKED EMPTY</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>CHECKED EMPTY</t>
-        </is>
-      </c>
-      <c r="E3" t="n">
-        <v>259538</v>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Clothing, Shoes &amp; Jewelry</t>
-        </is>
-      </c>
-      <c r="G3" t="n">
-        <v>635</v>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>Jewelry Trays</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="8" t="n">
-        <v>44309.62885515116</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>B08RYQ3JKD</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>CHECKED EMPTY</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>CHECKED EMPTY</t>
-        </is>
-      </c>
-      <c r="E4" t="n">
-        <v>259538</v>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Clothing, Shoes &amp; Jewelry</t>
-        </is>
-      </c>
-      <c r="G4" t="n">
-        <v>635</v>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>Jewelry Trays</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="8" t="n">
-        <v>44309.63194930273</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>B08RYQ3JKD</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>CHECKED EMPTY</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>CHECKED EMPTY</t>
-        </is>
-      </c>
-      <c r="E5" t="n">
-        <v>259538</v>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>Clothing, Shoes &amp; Jewelry</t>
-        </is>
-      </c>
-      <c r="G5" t="n">
-        <v>635</v>
-      </c>
-      <c r="H5" t="inlineStr">
         <is>
           <t>Jewelry Trays</t>
         </is>
@@ -5884,7 +3760,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5936,7 +3812,7 @@
     </row>
     <row r="2">
       <c r="A2" s="8" t="n">
-        <v>44309.62277303502</v>
+        <v>44309.69352162944</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -5954,7 +3830,7 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>584043</v>
+        <v>270604</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -5962,117 +3838,9 @@
         </is>
       </c>
       <c r="G2" t="n">
-        <v>1238</v>
+        <v>668</v>
       </c>
       <c r="H2" t="inlineStr">
-        <is>
-          <t>Jewelry Trays</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="8" t="n">
-        <v>44309.62411660443</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>B08RYPG2FS</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>CHECKED EMPTY</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>CHECKED EMPTY</t>
-        </is>
-      </c>
-      <c r="E3" t="n">
-        <v>584043</v>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Clothing, Shoes &amp; Jewelry</t>
-        </is>
-      </c>
-      <c r="G3" t="n">
-        <v>1238</v>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>Jewelry Trays</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="8" t="n">
-        <v>44309.62887488909</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>B08RYPG2FS</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>CHECKED EMPTY</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>CHECKED EMPTY</t>
-        </is>
-      </c>
-      <c r="E4" t="n">
-        <v>270604</v>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Clothing, Shoes &amp; Jewelry</t>
-        </is>
-      </c>
-      <c r="G4" t="n">
-        <v>668</v>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>Jewelry Trays</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="8" t="n">
-        <v>44309.63197170537</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>B08RYPG2FS</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>CHECKED EMPTY</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>CHECKED EMPTY</t>
-        </is>
-      </c>
-      <c r="E5" t="n">
-        <v>270604</v>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>Clothing, Shoes &amp; Jewelry</t>
-        </is>
-      </c>
-      <c r="G5" t="n">
-        <v>668</v>
-      </c>
-      <c r="H5" t="inlineStr">
         <is>
           <t>Jewelry Trays</t>
         </is>
@@ -6089,7 +3857,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6141,7 +3909,7 @@
     </row>
     <row r="2">
       <c r="A2" s="8" t="n">
-        <v>44309.62279170669</v>
+        <v>44309.69354048779</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -6159,7 +3927,7 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>679534</v>
+        <v>700031</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -6167,117 +3935,9 @@
         </is>
       </c>
       <c r="G2" t="n">
-        <v>1392</v>
+        <v>1424</v>
       </c>
       <c r="H2" t="inlineStr">
-        <is>
-          <t>Jewelry Trays</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="8" t="n">
-        <v>44309.62413356748</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>B08RYMVQVG</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>CHECKED EMPTY</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>CHECKED EMPTY</t>
-        </is>
-      </c>
-      <c r="E3" t="n">
-        <v>679534</v>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Clothing, Shoes &amp; Jewelry</t>
-        </is>
-      </c>
-      <c r="G3" t="n">
-        <v>1392</v>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>Jewelry Trays</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="8" t="n">
-        <v>44309.62889481064</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>B08RYMVQVG</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>CHECKED EMPTY</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>CHECKED EMPTY</t>
-        </is>
-      </c>
-      <c r="E4" t="n">
-        <v>700031</v>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Clothing, Shoes &amp; Jewelry</t>
-        </is>
-      </c>
-      <c r="G4" t="n">
-        <v>1424</v>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>Jewelry Trays</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="8" t="n">
-        <v>44309.63199066038</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>B08RYMVQVG</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>CHECKED EMPTY</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>CHECKED EMPTY</t>
-        </is>
-      </c>
-      <c r="E5" t="n">
-        <v>700031</v>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>Clothing, Shoes &amp; Jewelry</t>
-        </is>
-      </c>
-      <c r="G5" t="n">
-        <v>1424</v>
-      </c>
-      <c r="H5" t="inlineStr">
         <is>
           <t>Jewelry Trays</t>
         </is>
@@ -6294,7 +3954,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6346,7 +4006,7 @@
     </row>
     <row r="2">
       <c r="A2" s="8" t="n">
-        <v>44309.62281329244</v>
+        <v>44309.69356070193</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -6364,7 +4024,7 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>352022</v>
+        <v>124834</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -6372,117 +4032,9 @@
         </is>
       </c>
       <c r="G2" t="n">
-        <v>834</v>
+        <v>292</v>
       </c>
       <c r="H2" t="inlineStr">
-        <is>
-          <t>Jewelry Trays</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="8" t="n">
-        <v>44309.62415114735</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>B08RYQ4YVW</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>CHECKED EMPTY</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>CHECKED EMPTY</t>
-        </is>
-      </c>
-      <c r="E3" t="n">
-        <v>352022</v>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Clothing, Shoes &amp; Jewelry</t>
-        </is>
-      </c>
-      <c r="G3" t="n">
-        <v>834</v>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>Jewelry Trays</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="8" t="n">
-        <v>44309.6289156992</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>B08RYQ4YVW</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>CHECKED EMPTY</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>CHECKED EMPTY</t>
-        </is>
-      </c>
-      <c r="E4" t="n">
-        <v>124834</v>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Clothing, Shoes &amp; Jewelry</t>
-        </is>
-      </c>
-      <c r="G4" t="n">
-        <v>292</v>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>Jewelry Trays</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="8" t="n">
-        <v>44309.63201816849</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>B08RYQ4YVW</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>CHECKED EMPTY</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>CHECKED EMPTY</t>
-        </is>
-      </c>
-      <c r="E5" t="n">
-        <v>124834</v>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>Clothing, Shoes &amp; Jewelry</t>
-        </is>
-      </c>
-      <c r="G5" t="n">
-        <v>292</v>
-      </c>
-      <c r="H5" t="inlineStr">
         <is>
           <t>Jewelry Trays</t>
         </is>
@@ -6551,7 +4103,7 @@
     </row>
     <row r="2">
       <c r="A2" s="8" t="n">
-        <v>44309.63203850106</v>
+        <v>44309.69358004881</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -6652,7 +4204,7 @@
     </row>
     <row r="2">
       <c r="A2" s="8" t="n">
-        <v>44309.63205200678</v>
+        <v>44309.69359439487</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -6701,7 +4253,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6753,25 +4305,21 @@
     </row>
     <row r="2">
       <c r="A2" s="8" t="n">
-        <v>44309.62218803202</v>
+        <v>44309.69292205863</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
           <t>B07WWFWRJP</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>CHECKED EMPTY</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>CHECKED EMPTY</t>
-        </is>
+      <c r="C2" t="n">
+        <v>4.4</v>
+      </c>
+      <c r="D2" t="n">
+        <v>1650</v>
       </c>
       <c r="E2" t="n">
-        <v>84229</v>
+        <v>68308</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -6779,105 +4327,9 @@
         </is>
       </c>
       <c r="G2" t="n">
-        <v>323</v>
+        <v>284</v>
       </c>
       <c r="H2" t="inlineStr">
-        <is>
-          <t>Indoor String Lights</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="8" t="n">
-        <v>44309.62356151142</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>B07WWFWRJP</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>4.4</v>
-      </c>
-      <c r="D3" t="n">
-        <v>1649</v>
-      </c>
-      <c r="E3" t="n">
-        <v>68308</v>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Home &amp; Kitchen</t>
-        </is>
-      </c>
-      <c r="G3" t="n">
-        <v>284</v>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>Indoor String Lights</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="8" t="n">
-        <v>44309.62829406383</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>B07WWFWRJP</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>4.4</v>
-      </c>
-      <c r="D4" t="n">
-        <v>1649</v>
-      </c>
-      <c r="E4" t="n">
-        <v>68308</v>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Home &amp; Kitchen</t>
-        </is>
-      </c>
-      <c r="G4" t="n">
-        <v>284</v>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>Indoor String Lights</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="8" t="n">
-        <v>44309.6314126367</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>B07WWFWRJP</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>4.4</v>
-      </c>
-      <c r="D5" t="n">
-        <v>1649</v>
-      </c>
-      <c r="E5" t="n">
-        <v>68308</v>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>Home &amp; Kitchen</t>
-        </is>
-      </c>
-      <c r="G5" t="n">
-        <v>284</v>
-      </c>
-      <c r="H5" t="inlineStr">
         <is>
           <t>Indoor String Lights</t>
         </is>
@@ -6946,7 +4398,7 @@
     </row>
     <row r="2">
       <c r="A2" s="8" t="n">
-        <v>44309.63206822608</v>
+        <v>44309.69361213892</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -7047,7 +4499,7 @@
     </row>
     <row r="2">
       <c r="A2" s="8" t="n">
-        <v>44309.63208131991</v>
+        <v>44309.69362533696</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -7148,7 +4600,7 @@
     </row>
     <row r="2">
       <c r="A2" s="8" t="n">
-        <v>44309.63143338436</v>
+        <v>44309.69294466566</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -7249,7 +4701,7 @@
     </row>
     <row r="2">
       <c r="A2" s="8" t="n">
-        <v>44309.63144609342</v>
+        <v>44309.6929583357</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -7298,7 +4750,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7350,22 +4802,18 @@
     </row>
     <row r="2">
       <c r="A2" s="8" t="n">
-        <v>44309.6222404964</v>
+        <v>44309.6929712211</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
           <t>B07R5PCZLY</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>CHECKED EMPTY</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>CHECKED EMPTY</t>
-        </is>
+      <c r="C2" t="n">
+        <v>4.7</v>
+      </c>
+      <c r="D2" t="n">
+        <v>1003</v>
       </c>
       <c r="E2" t="n">
         <v>13441</v>
@@ -7379,102 +4827,6 @@
         <v>58</v>
       </c>
       <c r="H2" t="inlineStr">
-        <is>
-          <t>Serving Trays</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="8" t="n">
-        <v>44309.62360809729</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>B07R5PCZLY</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>4.7</v>
-      </c>
-      <c r="D3" t="n">
-        <v>1002</v>
-      </c>
-      <c r="E3" t="n">
-        <v>13441</v>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Kitchen &amp; Dining</t>
-        </is>
-      </c>
-      <c r="G3" t="n">
-        <v>58</v>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>Serving Trays</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="8" t="n">
-        <v>44309.62834217183</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>B07R5PCZLY</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>4.7</v>
-      </c>
-      <c r="D4" t="n">
-        <v>1002</v>
-      </c>
-      <c r="E4" t="n">
-        <v>13441</v>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Kitchen &amp; Dining</t>
-        </is>
-      </c>
-      <c r="G4" t="n">
-        <v>58</v>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>Serving Trays</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="8" t="n">
-        <v>44309.63146162183</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>B07R5PCZLY</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>4.7</v>
-      </c>
-      <c r="D5" t="n">
-        <v>1002</v>
-      </c>
-      <c r="E5" t="n">
-        <v>13441</v>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>Kitchen &amp; Dining</t>
-        </is>
-      </c>
-      <c r="G5" t="n">
-        <v>58</v>
-      </c>
-      <c r="H5" t="inlineStr">
         <is>
           <t>Serving Trays</t>
         </is>
@@ -7491,7 +4843,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7543,25 +4895,21 @@
     </row>
     <row r="2">
       <c r="A2" s="8" t="n">
-        <v>44309.6222649841</v>
+        <v>44309.69299679068</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
           <t>B087QD62HW</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>CHECKED EMPTY</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>CHECKED EMPTY</t>
-        </is>
+      <c r="C2" t="n">
+        <v>4.7</v>
+      </c>
+      <c r="D2" t="n">
+        <v>1003</v>
       </c>
       <c r="E2" t="n">
-        <v>12905</v>
+        <v>13441</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -7572,102 +4920,6 @@
         <v>58</v>
       </c>
       <c r="H2" t="inlineStr">
-        <is>
-          <t>Serving Trays</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="8" t="n">
-        <v>44309.62363243305</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>B087QD62HW</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>4.7</v>
-      </c>
-      <c r="D3" t="n">
-        <v>1002</v>
-      </c>
-      <c r="E3" t="n">
-        <v>12905</v>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Kitchen &amp; Dining</t>
-        </is>
-      </c>
-      <c r="G3" t="n">
-        <v>58</v>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>Serving Trays</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="8" t="n">
-        <v>44309.62836341342</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>B087QD62HW</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>4.7</v>
-      </c>
-      <c r="D4" t="n">
-        <v>1002</v>
-      </c>
-      <c r="E4" t="n">
-        <v>12905</v>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Kitchen &amp; Dining</t>
-        </is>
-      </c>
-      <c r="G4" t="n">
-        <v>58</v>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>Serving Trays</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="8" t="n">
-        <v>44309.63148821652</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>B087QD62HW</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>4.7</v>
-      </c>
-      <c r="D5" t="n">
-        <v>1002</v>
-      </c>
-      <c r="E5" t="n">
-        <v>13441</v>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>Kitchen &amp; Dining</t>
-        </is>
-      </c>
-      <c r="G5" t="n">
-        <v>58</v>
-      </c>
-      <c r="H5" t="inlineStr">
         <is>
           <t>Serving Trays</t>
         </is>
@@ -7684,7 +4936,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7736,22 +4988,18 @@
     </row>
     <row r="2">
       <c r="A2" s="8" t="n">
-        <v>44309.62228532729</v>
+        <v>44309.69301749542</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
           <t>B088RG7N5D</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>CHECKED EMPTY</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>CHECKED EMPTY</t>
-        </is>
+      <c r="C2" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="D2" t="n">
+        <v>237</v>
       </c>
       <c r="E2" t="n">
         <v>54725</v>
@@ -7765,102 +5013,6 @@
         <v>367</v>
       </c>
       <c r="H2" t="inlineStr">
-        <is>
-          <t>Serving Trays</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="8" t="n">
-        <v>44309.62365717655</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>B088RG7N5D</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>4.6</v>
-      </c>
-      <c r="D3" t="n">
-        <v>237</v>
-      </c>
-      <c r="E3" t="n">
-        <v>54725</v>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Kitchen &amp; Dining</t>
-        </is>
-      </c>
-      <c r="G3" t="n">
-        <v>367</v>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>Serving Trays</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="8" t="n">
-        <v>44309.62838385713</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>B088RG7N5D</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>4.6</v>
-      </c>
-      <c r="D4" t="n">
-        <v>237</v>
-      </c>
-      <c r="E4" t="n">
-        <v>54725</v>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Kitchen &amp; Dining</t>
-        </is>
-      </c>
-      <c r="G4" t="n">
-        <v>367</v>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>Serving Trays</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="8" t="n">
-        <v>44309.6315102744</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>B088RG7N5D</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>4.6</v>
-      </c>
-      <c r="D5" t="n">
-        <v>237</v>
-      </c>
-      <c r="E5" t="n">
-        <v>54725</v>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>Kitchen &amp; Dining</t>
-        </is>
-      </c>
-      <c r="G5" t="n">
-        <v>367</v>
-      </c>
-      <c r="H5" t="inlineStr">
         <is>
           <t>Serving Trays</t>
         </is>

</xml_diff>

<commit_message>
fix None page and better log
</commit_message>
<xml_diff>
--- a/EZDC.xlsx
+++ b/EZDC.xlsx
@@ -20,33 +20,30 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="B08R3HH8P8" sheetId="12" state="visible" r:id="rId12"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="B088RB1GRD" sheetId="13" state="visible" r:id="rId13"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="B08R3LN8NH" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="None" sheetId="15" state="visible" r:id="rId15"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="None1" sheetId="16" state="visible" r:id="rId16"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="None2" sheetId="17" state="visible" r:id="rId17"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="B087D7VP7B" sheetId="18" state="visible" r:id="rId18"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="B08RWTDF9W" sheetId="19" state="visible" r:id="rId19"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="B088RDY8YS" sheetId="20" state="visible" r:id="rId20"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="B088RD9XK6" sheetId="21" state="visible" r:id="rId21"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="B088RC9TNP" sheetId="22" state="visible" r:id="rId22"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="B092MHYBPS" sheetId="23" state="visible" r:id="rId23"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="B092MK78G2" sheetId="24" state="visible" r:id="rId24"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="B092MKSB54" sheetId="25" state="visible" r:id="rId25"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="B092ML7MW1" sheetId="26" state="visible" r:id="rId26"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="B08RDDR92G" sheetId="27" state="visible" r:id="rId27"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="B08RDCBV6V" sheetId="28" state="visible" r:id="rId28"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="B08RJ7S3Y5" sheetId="29" state="visible" r:id="rId29"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="B08RJG6YMP" sheetId="30" state="visible" r:id="rId30"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="B08RYPRTTF" sheetId="31" state="visible" r:id="rId31"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="B08RYQX56M" sheetId="32" state="visible" r:id="rId32"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="B08RYN4M1J" sheetId="33" state="visible" r:id="rId33"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="B08RYQ3JKD" sheetId="34" state="visible" r:id="rId34"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="B08RYPG2FS" sheetId="35" state="visible" r:id="rId35"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="B08RYMVQVG" sheetId="36" state="visible" r:id="rId36"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="B08RYQ4YVW" sheetId="37" state="visible" r:id="rId37"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="B08Z3CSCFR" sheetId="38" state="visible" r:id="rId38"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="B08Z3GRY4K" sheetId="39" state="visible" r:id="rId39"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="B08Z3CTCCZ" sheetId="40" state="visible" r:id="rId40"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="B08Z37PD7L" sheetId="41" state="visible" r:id="rId41"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="B087D7VP7B" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="B08RWTDF9W" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="B088RDY8YS" sheetId="17" state="visible" r:id="rId17"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="B088RD9XK6" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="B088RC9TNP" sheetId="19" state="visible" r:id="rId19"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="B092MHYBPS" sheetId="20" state="visible" r:id="rId20"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="B092MK78G2" sheetId="21" state="visible" r:id="rId21"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="B092MKSB54" sheetId="22" state="visible" r:id="rId22"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="B092ML7MW1" sheetId="23" state="visible" r:id="rId23"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="B08RDDR92G" sheetId="24" state="visible" r:id="rId24"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="B08RDCBV6V" sheetId="25" state="visible" r:id="rId25"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="B08RJ7S3Y5" sheetId="26" state="visible" r:id="rId26"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="B08RJG6YMP" sheetId="27" state="visible" r:id="rId27"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="B08RYPRTTF" sheetId="28" state="visible" r:id="rId28"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="B08RYQX56M" sheetId="29" state="visible" r:id="rId29"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="B08RYN4M1J" sheetId="30" state="visible" r:id="rId30"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="B08RYQ3JKD" sheetId="31" state="visible" r:id="rId31"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="B08RYPG2FS" sheetId="32" state="visible" r:id="rId32"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="B08RYMVQVG" sheetId="33" state="visible" r:id="rId33"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="B08RYQ4YVW" sheetId="34" state="visible" r:id="rId34"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="B08Z3CSCFR" sheetId="35" state="visible" r:id="rId35"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="B08Z3GRY4K" sheetId="36" state="visible" r:id="rId36"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="B08Z3CTCCZ" sheetId="37" state="visible" r:id="rId37"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="B08Z37PD7L" sheetId="38" state="visible" r:id="rId38"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="162913" fullCalcOnLoad="1"/>
@@ -1189,7 +1186,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1241,7 +1238,7 @@
     </row>
     <row r="2">
       <c r="A2" s="8" t="n">
-        <v>44309.69303853926</v>
+        <v>44311.59810900691</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -1255,7 +1252,7 @@
         <v>237</v>
       </c>
       <c r="E2" t="n">
-        <v>54725</v>
+        <v>73336</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -1263,9 +1260,41 @@
         </is>
       </c>
       <c r="G2" t="n">
-        <v>367</v>
+        <v>554</v>
       </c>
       <c r="H2" t="inlineStr">
+        <is>
+          <t>Serving Trays</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="8" t="n">
+        <v>44311.60588833033</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>B088RG7N5D</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="D3" t="n">
+        <v>237</v>
+      </c>
+      <c r="E3" t="n">
+        <v>73336</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Kitchen &amp; Dining</t>
+        </is>
+      </c>
+      <c r="G3" t="n">
+        <v>554</v>
+      </c>
+      <c r="H3" t="inlineStr">
         <is>
           <t>Serving Trays</t>
         </is>
@@ -1282,7 +1311,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1334,7 +1363,7 @@
     </row>
     <row r="2">
       <c r="A2" s="8" t="n">
-        <v>44309.69305795074</v>
+        <v>44311.5981302016</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -1348,7 +1377,7 @@
         <v>2</v>
       </c>
       <c r="E2" t="n">
-        <v>72726</v>
+        <v>81649</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -1356,9 +1385,41 @@
         </is>
       </c>
       <c r="G2" t="n">
-        <v>518</v>
+        <v>619</v>
       </c>
       <c r="H2" t="inlineStr">
+        <is>
+          <t>Serving Trays</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="8" t="n">
+        <v>44311.60591018593</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>B08R3HNBMF</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="D3" t="n">
+        <v>2</v>
+      </c>
+      <c r="E3" t="n">
+        <v>81649</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Kitchen &amp; Dining</t>
+        </is>
+      </c>
+      <c r="G3" t="n">
+        <v>619</v>
+      </c>
+      <c r="H3" t="inlineStr">
         <is>
           <t>Serving Trays</t>
         </is>
@@ -1375,7 +1436,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1427,7 +1488,7 @@
     </row>
     <row r="2">
       <c r="A2" s="8" t="n">
-        <v>44309.69308349252</v>
+        <v>44311.59815187737</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -1441,7 +1502,7 @@
         <v>2</v>
       </c>
       <c r="E2" t="n">
-        <v>72726</v>
+        <v>81649</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -1449,9 +1510,41 @@
         </is>
       </c>
       <c r="G2" t="n">
-        <v>518</v>
+        <v>619</v>
       </c>
       <c r="H2" t="inlineStr">
+        <is>
+          <t>Serving Trays</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="8" t="n">
+        <v>44311.60592872191</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>B08R3HH8P8</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="D3" t="n">
+        <v>2</v>
+      </c>
+      <c r="E3" t="n">
+        <v>81649</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Kitchen &amp; Dining</t>
+        </is>
+      </c>
+      <c r="G3" t="n">
+        <v>619</v>
+      </c>
+      <c r="H3" t="inlineStr">
         <is>
           <t>Serving Trays</t>
         </is>
@@ -1468,7 +1561,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1520,7 +1613,7 @@
     </row>
     <row r="2">
       <c r="A2" s="8" t="n">
-        <v>44309.6931038873</v>
+        <v>44311.598171935</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -1531,10 +1624,10 @@
         <v>4.4</v>
       </c>
       <c r="D2" t="n">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="E2" t="n">
-        <v>81452</v>
+        <v>72530</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -1542,9 +1635,41 @@
         </is>
       </c>
       <c r="G2" t="n">
-        <v>106</v>
+        <v>74</v>
       </c>
       <c r="H2" t="inlineStr">
+        <is>
+          <t>Decorative Boxes</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="8" t="n">
+        <v>44311.60595207435</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>B088RB1GRD</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>4.4</v>
+      </c>
+      <c r="D3" t="n">
+        <v>172</v>
+      </c>
+      <c r="E3" t="n">
+        <v>72530</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Home &amp; Kitchen</t>
+        </is>
+      </c>
+      <c r="G3" t="n">
+        <v>74</v>
+      </c>
+      <c r="H3" t="inlineStr">
         <is>
           <t>Decorative Boxes</t>
         </is>
@@ -1561,7 +1686,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1613,7 +1738,7 @@
     </row>
     <row r="2">
       <c r="A2" s="8" t="n">
-        <v>44309.69312686843</v>
+        <v>44311.59819328944</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -1627,7 +1752,7 @@
         <v>11</v>
       </c>
       <c r="E2" t="n">
-        <v>166014</v>
+        <v>168771</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -1635,11 +1760,283 @@
         </is>
       </c>
       <c r="G2" t="n">
-        <v>683</v>
+        <v>677</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
           <t>Floating Shelves</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="8" t="n">
+        <v>44311.59821728521</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="8" t="n">
+        <v>44311.5982199697</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="8" t="n">
+        <v>44311.59822264417</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="8" t="n">
+        <v>44311.60597241564</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>B08R3LN8NH</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>4.3</v>
+      </c>
+      <c r="D6" t="n">
+        <v>11</v>
+      </c>
+      <c r="E6" t="n">
+        <v>168771</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Home &amp; Kitchen</t>
+        </is>
+      </c>
+      <c r="G6" t="n">
+        <v>677</v>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Floating Shelves</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="8" t="n">
+        <v>44311.6059902645</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="8" t="n">
+        <v>44311.60599368913</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="8" t="n">
+        <v>44311.60599685276</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>NAN</t>
         </is>
       </c>
     </row>
@@ -1654,7 +2051,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1706,41 +2103,65 @@
     </row>
     <row r="2">
       <c r="A2" s="8" t="n">
-        <v>44309.69315105717</v>
+        <v>44311.59822532607</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>NAN</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>NAN</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>NAN</t>
-        </is>
+          <t>B087D7VP7B</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="D2" t="n">
+        <v>165</v>
+      </c>
+      <c r="E2" t="n">
+        <v>168786</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>NAN</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>NAN</t>
-        </is>
+          <t>Home &amp; Kitchen</t>
+        </is>
+      </c>
+      <c r="G2" t="n">
+        <v>112</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>NAN</t>
+          <t>Decorative Trays</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="8" t="n">
+        <v>44311.60600002538</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>B087D7VP7B</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="D3" t="n">
+        <v>165</v>
+      </c>
+      <c r="E3" t="n">
+        <v>168786</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Home &amp; Kitchen</t>
+        </is>
+      </c>
+      <c r="G3" t="n">
+        <v>112</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Decorative Trays</t>
         </is>
       </c>
     </row>
@@ -1755,7 +2176,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1807,41 +2228,65 @@
     </row>
     <row r="2">
       <c r="A2" s="8" t="n">
-        <v>44309.69315424914</v>
+        <v>44311.59824782874</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>NAN</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>NAN</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>NAN</t>
-        </is>
+          <t>B087D7VP7B</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="D2" t="n">
+        <v>165</v>
+      </c>
+      <c r="E2" t="n">
+        <v>168786</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>NAN</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>NAN</t>
-        </is>
+          <t>Home &amp; Kitchen</t>
+        </is>
+      </c>
+      <c r="G2" t="n">
+        <v>112</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>NAN</t>
+          <t>Decorative Trays</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="8" t="n">
+        <v>44311.60602093848</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>B087D7VP7B</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="D3" t="n">
+        <v>165</v>
+      </c>
+      <c r="E3" t="n">
+        <v>168786</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Home &amp; Kitchen</t>
+        </is>
+      </c>
+      <c r="G3" t="n">
+        <v>112</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Decorative Trays</t>
         </is>
       </c>
     </row>
@@ -1856,7 +2301,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1908,41 +2353,65 @@
     </row>
     <row r="2">
       <c r="A2" s="8" t="n">
-        <v>44309.69315731672</v>
+        <v>44311.59826655109</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>NAN</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>NAN</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>NAN</t>
-        </is>
+          <t>B088RDY8YS</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="D2" t="n">
+        <v>127</v>
+      </c>
+      <c r="E2" t="n">
+        <v>336420</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>NAN</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>NAN</t>
-        </is>
+          <t>Home &amp; Kitchen</t>
+        </is>
+      </c>
+      <c r="G2" t="n">
+        <v>38</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>NAN</t>
+          <t>Sculptural Picture Frames &amp; Holders</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="8" t="n">
+        <v>44311.60604019935</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>B088RDY8YS</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="D3" t="n">
+        <v>127</v>
+      </c>
+      <c r="E3" t="n">
+        <v>336420</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Home &amp; Kitchen</t>
+        </is>
+      </c>
+      <c r="G3" t="n">
+        <v>38</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Sculptural Picture Frames &amp; Holders</t>
         </is>
       </c>
     </row>
@@ -1957,7 +2426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2009,21 +2478,21 @@
     </row>
     <row r="2">
       <c r="A2" s="8" t="n">
-        <v>44309.69316040542</v>
+        <v>44311.59828897219</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>B087D7VP7B</t>
+          <t>B088RD9XK6</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>4.6</v>
+        <v>4.7</v>
       </c>
       <c r="D2" t="n">
-        <v>163</v>
+        <v>59</v>
       </c>
       <c r="E2" t="n">
-        <v>206436</v>
+        <v>72274</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -2031,11 +2500,43 @@
         </is>
       </c>
       <c r="G2" t="n">
-        <v>149</v>
+        <v>17</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Decorative Trays</t>
+          <t>Decorative Bookends</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="8" t="n">
+        <v>44311.60605984653</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>B088RD9XK6</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>4.7</v>
+      </c>
+      <c r="D3" t="n">
+        <v>59</v>
+      </c>
+      <c r="E3" t="n">
+        <v>72274</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Home &amp; Kitchen</t>
+        </is>
+      </c>
+      <c r="G3" t="n">
+        <v>17</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Decorative Bookends</t>
         </is>
       </c>
     </row>
@@ -2050,7 +2551,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2102,21 +2603,21 @@
     </row>
     <row r="2">
       <c r="A2" s="8" t="n">
-        <v>44309.69318463845</v>
+        <v>44311.59831218972</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>B087D7VP7B</t>
+          <t>B088RC9TNP</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>4.6</v>
+        <v>4.7</v>
       </c>
       <c r="D2" t="n">
-        <v>163</v>
+        <v>59</v>
       </c>
       <c r="E2" t="n">
-        <v>206436</v>
+        <v>72274</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -2124,11 +2625,43 @@
         </is>
       </c>
       <c r="G2" t="n">
-        <v>149</v>
+        <v>17</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Decorative Trays</t>
+          <t>Decorative Bookends</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="8" t="n">
+        <v>44311.60608054867</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>B088RC9TNP</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>4.7</v>
+      </c>
+      <c r="D3" t="n">
+        <v>59</v>
+      </c>
+      <c r="E3" t="n">
+        <v>72274</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Home &amp; Kitchen</t>
+        </is>
+      </c>
+      <c r="G3" t="n">
+        <v>17</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Decorative Bookends</t>
         </is>
       </c>
     </row>
@@ -2143,7 +2676,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2195,7 +2728,7 @@
     </row>
     <row r="2">
       <c r="A2" s="8" t="n">
-        <v>44309.6928730228</v>
+        <v>44311.59794825426</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -2209,7 +2742,7 @@
         <v>1650</v>
       </c>
       <c r="E2" t="n">
-        <v>68308</v>
+        <v>55033</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -2217,9 +2750,41 @@
         </is>
       </c>
       <c r="G2" t="n">
-        <v>284</v>
+        <v>218</v>
       </c>
       <c r="H2" t="inlineStr">
+        <is>
+          <t>Indoor String Lights</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="8" t="n">
+        <v>44311.60572597438</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>B07F6YFT4F</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>4.4</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1650</v>
+      </c>
+      <c r="E3" t="n">
+        <v>55033</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Home &amp; Kitchen</t>
+        </is>
+      </c>
+      <c r="G3" t="n">
+        <v>218</v>
+      </c>
+      <c r="H3" t="inlineStr">
         <is>
           <t>Indoor String Lights</t>
         </is>
@@ -2236,7 +2801,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2288,21 +2853,21 @@
     </row>
     <row r="2">
       <c r="A2" s="8" t="n">
-        <v>44309.69320218355</v>
+        <v>44311.59833349768</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>B088RDY8YS</t>
+          <t>B088RD9XK6</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>4.5</v>
+        <v>4.7</v>
       </c>
       <c r="D2" t="n">
-        <v>127</v>
+        <v>59</v>
       </c>
       <c r="E2" t="n">
-        <v>196384</v>
+        <v>72274</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -2310,11 +2875,43 @@
         </is>
       </c>
       <c r="G2" t="n">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Sculptural Picture Frames &amp; Holders</t>
+          <t>Decorative Bookends</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="8" t="n">
+        <v>44311.60609937383</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>B088RD9XK6</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>4.7</v>
+      </c>
+      <c r="D3" t="n">
+        <v>59</v>
+      </c>
+      <c r="E3" t="n">
+        <v>72274</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Home &amp; Kitchen</t>
+        </is>
+      </c>
+      <c r="G3" t="n">
+        <v>17</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Decorative Bookends</t>
         </is>
       </c>
     </row>
@@ -2329,7 +2926,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2381,33 +2978,81 @@
     </row>
     <row r="2">
       <c r="A2" s="8" t="n">
-        <v>44309.69322519479</v>
+        <v>44311.59835286144</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>B088RD9XK6</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>4.7</v>
-      </c>
-      <c r="D2" t="n">
-        <v>58</v>
-      </c>
-      <c r="E2" t="n">
-        <v>83260</v>
+          <t>B092MK78G2</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Home &amp; Kitchen</t>
-        </is>
-      </c>
-      <c r="G2" t="n">
-        <v>16</v>
+          <t>NAN</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Decorative Bookends</t>
+          <t>NAN</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="8" t="n">
+        <v>44311.60612021392</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>B092MK78G2</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>NAN</t>
         </is>
       </c>
     </row>
@@ -2422,7 +3067,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2474,33 +3119,81 @@
     </row>
     <row r="2">
       <c r="A2" s="8" t="n">
-        <v>44309.69324976933</v>
+        <v>44311.59836630892</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>B088RC9TNP</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>4.7</v>
-      </c>
-      <c r="D2" t="n">
-        <v>58</v>
-      </c>
-      <c r="E2" t="n">
-        <v>83260</v>
+          <t>B092MKSB54</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Home &amp; Kitchen</t>
-        </is>
-      </c>
-      <c r="G2" t="n">
-        <v>16</v>
+          <t>NAN</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Decorative Bookends</t>
+          <t>NAN</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="8" t="n">
+        <v>44311.60613343497</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>B092MKSB54</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>NAN</t>
         </is>
       </c>
     </row>
@@ -2515,7 +3208,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2567,33 +3260,81 @@
     </row>
     <row r="2">
       <c r="A2" s="8" t="n">
-        <v>44309.69327036794</v>
+        <v>44311.59837951195</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>B088RD9XK6</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>4.7</v>
-      </c>
-      <c r="D2" t="n">
-        <v>58</v>
-      </c>
-      <c r="E2" t="n">
-        <v>83260</v>
+          <t>B092ML7MW1</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Home &amp; Kitchen</t>
-        </is>
-      </c>
-      <c r="G2" t="n">
-        <v>16</v>
+          <t>NAN</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Decorative Bookends</t>
+          <t>NAN</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="8" t="n">
+        <v>44311.60614698922</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>B092ML7MW1</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>NAN</t>
         </is>
       </c>
     </row>
@@ -2608,7 +3349,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2660,41 +3401,65 @@
     </row>
     <row r="2">
       <c r="A2" s="8" t="n">
-        <v>44309.69329471978</v>
+        <v>44311.59839325473</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>B092MK78G2</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>NAN</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>NAN</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>NAN</t>
-        </is>
+          <t>B08RDDR92G</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>3.9</v>
+      </c>
+      <c r="D2" t="n">
+        <v>10</v>
+      </c>
+      <c r="E2" t="n">
+        <v>82045</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>NAN</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>NAN</t>
-        </is>
+          <t>Home &amp; Kitchen</t>
+        </is>
+      </c>
+      <c r="G2" t="n">
+        <v>444</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>NAN</t>
+          <t>Artificial Plants &amp; Greenery</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="8" t="n">
+        <v>44311.60616206273</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>B08RDDR92G</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>3.9</v>
+      </c>
+      <c r="D3" t="n">
+        <v>10</v>
+      </c>
+      <c r="E3" t="n">
+        <v>82045</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Home &amp; Kitchen</t>
+        </is>
+      </c>
+      <c r="G3" t="n">
+        <v>444</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Artificial Plants &amp; Greenery</t>
         </is>
       </c>
     </row>
@@ -2709,7 +3474,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2761,41 +3526,65 @@
     </row>
     <row r="2">
       <c r="A2" s="8" t="n">
-        <v>44309.69330698111</v>
+        <v>44311.59841266485</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>B092MKSB54</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>NAN</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>NAN</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>NAN</t>
-        </is>
+          <t>B08RDCBV6V</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>3.9</v>
+      </c>
+      <c r="D2" t="n">
+        <v>10</v>
+      </c>
+      <c r="E2" t="n">
+        <v>82045</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>NAN</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>NAN</t>
-        </is>
+          <t>Home &amp; Kitchen</t>
+        </is>
+      </c>
+      <c r="G2" t="n">
+        <v>444</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>NAN</t>
+          <t>Artificial Plants &amp; Greenery</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="8" t="n">
+        <v>44311.60618122464</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>B08RDCBV6V</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>3.9</v>
+      </c>
+      <c r="D3" t="n">
+        <v>10</v>
+      </c>
+      <c r="E3" t="n">
+        <v>82045</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Home &amp; Kitchen</t>
+        </is>
+      </c>
+      <c r="G3" t="n">
+        <v>444</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Artificial Plants &amp; Greenery</t>
         </is>
       </c>
     </row>
@@ -2810,7 +3599,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2862,41 +3651,65 @@
     </row>
     <row r="2">
       <c r="A2" s="8" t="n">
-        <v>44309.69331913685</v>
+        <v>44311.59843317234</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>B092ML7MW1</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>NAN</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>NAN</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>NAN</t>
-        </is>
+          <t>B08RJ7S3Y5</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D2" t="n">
+        <v>6</v>
+      </c>
+      <c r="E2" t="n">
+        <v>172574</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>NAN</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>NAN</t>
-        </is>
+          <t>Home &amp; Kitchen</t>
+        </is>
+      </c>
+      <c r="G2" t="n">
+        <v>1787</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>NAN</t>
+          <t>Artificial Flowers</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="8" t="n">
+        <v>44311.60619933795</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>B08RJ7S3Y5</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>2</v>
+      </c>
+      <c r="D3" t="n">
+        <v>6</v>
+      </c>
+      <c r="E3" t="n">
+        <v>150695</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Home &amp; Kitchen</t>
+        </is>
+      </c>
+      <c r="G3" t="n">
+        <v>1584</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Artificial Flowers</t>
         </is>
       </c>
     </row>
@@ -2911,7 +3724,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2963,21 +3776,21 @@
     </row>
     <row r="2">
       <c r="A2" s="8" t="n">
-        <v>44309.69333142805</v>
+        <v>44311.59845713431</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>B08RDDR92G</t>
+          <t>B08RJG6YMP</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>3.8</v>
+        <v>2</v>
       </c>
       <c r="D2" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E2" t="n">
-        <v>63280</v>
+        <v>150695</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -2985,11 +3798,43 @@
         </is>
       </c>
       <c r="G2" t="n">
-        <v>352</v>
+        <v>1584</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Artificial Plants &amp; Greenery</t>
+          <t>Artificial Flowers</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="8" t="n">
+        <v>44311.60621788035</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>B08RJG6YMP</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>2</v>
+      </c>
+      <c r="D3" t="n">
+        <v>6</v>
+      </c>
+      <c r="E3" t="n">
+        <v>150695</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Home &amp; Kitchen</t>
+        </is>
+      </c>
+      <c r="G3" t="n">
+        <v>1584</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Artificial Flowers</t>
         </is>
       </c>
     </row>
@@ -3004,7 +3849,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3056,33 +3901,73 @@
     </row>
     <row r="2">
       <c r="A2" s="8" t="n">
-        <v>44309.69335371384</v>
+        <v>44311.59847546839</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>B08RDCBV6V</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>3.8</v>
-      </c>
-      <c r="D2" t="n">
-        <v>9</v>
+          <t>B08RYPRTTF</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>CHECKED EMPTY</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>CHECKED EMPTY</t>
+        </is>
       </c>
       <c r="E2" t="n">
-        <v>63280</v>
+        <v>144452</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Home &amp; Kitchen</t>
+          <t>Clothing, Shoes &amp; Jewelry</t>
         </is>
       </c>
       <c r="G2" t="n">
-        <v>352</v>
+        <v>358</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Artificial Plants &amp; Greenery</t>
+          <t>Jewelry Trays</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="8" t="n">
+        <v>44311.60623623343</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>B08RYPRTTF</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>CHECKED EMPTY</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>CHECKED EMPTY</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>144452</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Clothing, Shoes &amp; Jewelry</t>
+        </is>
+      </c>
+      <c r="G3" t="n">
+        <v>358</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Jewelry Trays</t>
         </is>
       </c>
     </row>
@@ -3097,7 +3982,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3149,33 +4034,73 @@
     </row>
     <row r="2">
       <c r="A2" s="8" t="n">
-        <v>44309.69337152607</v>
+        <v>44311.59849691492</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>B08RJ7S3Y5</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>2</v>
-      </c>
-      <c r="D2" t="n">
-        <v>6</v>
+          <t>B08RYQX56M</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>CHECKED EMPTY</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>CHECKED EMPTY</t>
+        </is>
       </c>
       <c r="E2" t="n">
-        <v>130805</v>
+        <v>144452</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Home &amp; Kitchen</t>
+          <t>Clothing, Shoes &amp; Jewelry</t>
         </is>
       </c>
       <c r="G2" t="n">
-        <v>1413</v>
+        <v>358</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Artificial Flowers</t>
+          <t>Jewelry Trays</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="8" t="n">
+        <v>44311.60625314835</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>B08RYQX56M</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>CHECKED EMPTY</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>CHECKED EMPTY</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>144452</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Clothing, Shoes &amp; Jewelry</t>
+        </is>
+      </c>
+      <c r="G3" t="n">
+        <v>358</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Jewelry Trays</t>
         </is>
       </c>
     </row>
@@ -3190,7 +4115,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3242,7 +4167,7 @@
     </row>
     <row r="2">
       <c r="A2" s="8" t="n">
-        <v>44309.69290122313</v>
+        <v>44311.59797266489</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -3256,7 +4181,7 @@
         <v>1650</v>
       </c>
       <c r="E2" t="n">
-        <v>68308</v>
+        <v>55033</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -3264,9 +4189,41 @@
         </is>
       </c>
       <c r="G2" t="n">
-        <v>284</v>
+        <v>218</v>
       </c>
       <c r="H2" t="inlineStr">
+        <is>
+          <t>Indoor String Lights</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="8" t="n">
+        <v>44311.60575119727</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>B07F1FWK43</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>4.4</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1650</v>
+      </c>
+      <c r="E3" t="n">
+        <v>55033</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Home &amp; Kitchen</t>
+        </is>
+      </c>
+      <c r="G3" t="n">
+        <v>218</v>
+      </c>
+      <c r="H3" t="inlineStr">
         <is>
           <t>Indoor String Lights</t>
         </is>
@@ -3283,7 +4240,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3335,33 +4292,65 @@
     </row>
     <row r="2">
       <c r="A2" s="8" t="n">
-        <v>44309.69339237434</v>
+        <v>44311.5985160902</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>B08RJG6YMP</t>
+          <t>B08RYN4M1J</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D2" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E2" t="n">
-        <v>130805</v>
+        <v>122425</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Home &amp; Kitchen</t>
+          <t>Clothing, Shoes &amp; Jewelry</t>
         </is>
       </c>
       <c r="G2" t="n">
-        <v>1413</v>
+        <v>288</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Artificial Flowers</t>
+          <t>Jewelry Trays</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="8" t="n">
+        <v>44311.60627188379</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>B08RYN4M1J</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>5</v>
+      </c>
+      <c r="D3" t="n">
+        <v>3</v>
+      </c>
+      <c r="E3" t="n">
+        <v>122425</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Clothing, Shoes &amp; Jewelry</t>
+        </is>
+      </c>
+      <c r="G3" t="n">
+        <v>288</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Jewelry Trays</t>
         </is>
       </c>
     </row>
@@ -3376,7 +4365,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3428,11 +4417,11 @@
     </row>
     <row r="2">
       <c r="A2" s="8" t="n">
-        <v>44309.69341404419</v>
+        <v>44311.59853588218</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>B08RYPRTTF</t>
+          <t>B08RYQ3JKD</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -3446,7 +4435,7 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>152958</v>
+        <v>270193</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -3454,9 +4443,45 @@
         </is>
       </c>
       <c r="G2" t="n">
-        <v>363</v>
+        <v>684</v>
       </c>
       <c r="H2" t="inlineStr">
+        <is>
+          <t>Jewelry Trays</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="8" t="n">
+        <v>44311.60628882481</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>B08RYQ3JKD</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>CHECKED EMPTY</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>CHECKED EMPTY</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>270193</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Clothing, Shoes &amp; Jewelry</t>
+        </is>
+      </c>
+      <c r="G3" t="n">
+        <v>684</v>
+      </c>
+      <c r="H3" t="inlineStr">
         <is>
           <t>Jewelry Trays</t>
         </is>
@@ -3473,7 +4498,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3525,11 +4550,11 @@
     </row>
     <row r="2">
       <c r="A2" s="8" t="n">
-        <v>44309.69343968834</v>
+        <v>44311.5985574906</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>B08RYQX56M</t>
+          <t>B08RYPG2FS</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -3543,7 +4568,7 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>152958</v>
+        <v>240790</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -3551,9 +4576,45 @@
         </is>
       </c>
       <c r="G2" t="n">
-        <v>363</v>
+        <v>605</v>
       </c>
       <c r="H2" t="inlineStr">
+        <is>
+          <t>Jewelry Trays</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="8" t="n">
+        <v>44311.60630626928</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>B08RYPG2FS</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>CHECKED EMPTY</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>CHECKED EMPTY</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>240790</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Clothing, Shoes &amp; Jewelry</t>
+        </is>
+      </c>
+      <c r="G3" t="n">
+        <v>605</v>
+      </c>
+      <c r="H3" t="inlineStr">
         <is>
           <t>Jewelry Trays</t>
         </is>
@@ -3570,7 +4631,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3622,21 +4683,25 @@
     </row>
     <row r="2">
       <c r="A2" s="8" t="n">
-        <v>44309.69346341551</v>
+        <v>44311.59857591606</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>B08RYN4M1J</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>5</v>
-      </c>
-      <c r="D2" t="n">
-        <v>3</v>
+          <t>B08RYMVQVG</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>CHECKED EMPTY</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>CHECKED EMPTY</t>
+        </is>
       </c>
       <c r="E2" t="n">
-        <v>122059</v>
+        <v>531544</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -3644,9 +4709,45 @@
         </is>
       </c>
       <c r="G2" t="n">
-        <v>282</v>
+        <v>1144</v>
       </c>
       <c r="H2" t="inlineStr">
+        <is>
+          <t>Jewelry Trays</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="8" t="n">
+        <v>44311.60632234129</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>B08RYMVQVG</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>CHECKED EMPTY</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>CHECKED EMPTY</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>261049</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Clothing, Shoes &amp; Jewelry</t>
+        </is>
+      </c>
+      <c r="G3" t="n">
+        <v>665</v>
+      </c>
+      <c r="H3" t="inlineStr">
         <is>
           <t>Jewelry Trays</t>
         </is>
@@ -3663,7 +4764,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3715,25 +4816,21 @@
     </row>
     <row r="2">
       <c r="A2" s="8" t="n">
-        <v>44309.69349871631</v>
+        <v>44311.59859738658</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>B08RYQ3JKD</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>CHECKED EMPTY</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>CHECKED EMPTY</t>
-        </is>
+          <t>B08RYQ4YVW</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>5</v>
+      </c>
+      <c r="D2" t="n">
+        <v>1</v>
       </c>
       <c r="E2" t="n">
-        <v>307550</v>
+        <v>303075</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -3741,9 +4838,41 @@
         </is>
       </c>
       <c r="G2" t="n">
-        <v>745</v>
+        <v>730</v>
       </c>
       <c r="H2" t="inlineStr">
+        <is>
+          <t>Jewelry Trays</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="8" t="n">
+        <v>44311.606338371</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>B08RYQ4YVW</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>5</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" t="n">
+        <v>190170</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Clothing, Shoes &amp; Jewelry</t>
+        </is>
+      </c>
+      <c r="G3" t="n">
+        <v>478</v>
+      </c>
+      <c r="H3" t="inlineStr">
         <is>
           <t>Jewelry Trays</t>
         </is>
@@ -3760,7 +4889,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3812,37 +4941,81 @@
     </row>
     <row r="2">
       <c r="A2" s="8" t="n">
-        <v>44309.69352162944</v>
+        <v>44311.59861696974</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>B08RYPG2FS</t>
+          <t>B08Z3CSCFR</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>CHECKED EMPTY</t>
+          <t>NAN</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>CHECKED EMPTY</t>
-        </is>
-      </c>
-      <c r="E2" t="n">
-        <v>270604</v>
+          <t>NAN</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Clothing, Shoes &amp; Jewelry</t>
-        </is>
-      </c>
-      <c r="G2" t="n">
-        <v>668</v>
+          <t>NAN</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Jewelry Trays</t>
+          <t>NAN</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="8" t="n">
+        <v>44311.60635446409</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>B08Z3CSCFR</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>NAN</t>
         </is>
       </c>
     </row>
@@ -3857,7 +5030,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3909,37 +5082,81 @@
     </row>
     <row r="2">
       <c r="A2" s="8" t="n">
-        <v>44309.69354048779</v>
+        <v>44311.59863014094</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>B08RYMVQVG</t>
+          <t>B08Z3GRY4K</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>CHECKED EMPTY</t>
+          <t>NAN</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>CHECKED EMPTY</t>
-        </is>
-      </c>
-      <c r="E2" t="n">
-        <v>700031</v>
+          <t>NAN</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Clothing, Shoes &amp; Jewelry</t>
-        </is>
-      </c>
-      <c r="G2" t="n">
-        <v>1424</v>
+          <t>NAN</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Jewelry Trays</t>
+          <t>NAN</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="8" t="n">
+        <v>44311.60636839731</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>B08Z3GRY4K</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>NAN</t>
         </is>
       </c>
     </row>
@@ -3954,7 +5171,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4006,37 +5223,81 @@
     </row>
     <row r="2">
       <c r="A2" s="8" t="n">
-        <v>44309.69356070193</v>
+        <v>44311.59865424984</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>B08RYQ4YVW</t>
+          <t>B08Z3CTCCZ</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>CHECKED EMPTY</t>
+          <t>NAN</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>CHECKED EMPTY</t>
-        </is>
-      </c>
-      <c r="E2" t="n">
-        <v>124834</v>
+          <t>NAN</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Clothing, Shoes &amp; Jewelry</t>
-        </is>
-      </c>
-      <c r="G2" t="n">
-        <v>292</v>
+          <t>NAN</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Jewelry Trays</t>
+          <t>NAN</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="8" t="n">
+        <v>44311.60638410589</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>B08Z3CTCCZ</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>NAN</t>
         </is>
       </c>
     </row>
@@ -4051,7 +5312,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4103,11 +5364,11 @@
     </row>
     <row r="2">
       <c r="A2" s="8" t="n">
-        <v>44309.69358004881</v>
+        <v>44311.59866989798</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>B08Z3CSCFR</t>
+          <t>B08Z37PD7L</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -4141,102 +5402,41 @@
         </is>
       </c>
     </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:H2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Date</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>ASIN</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>STARS</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>NUM_RATING</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>RANKING1</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>RANKING1_CAT</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>RANKING2</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>RANKING2_CAT</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="8" t="n">
-        <v>44309.69359439487</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>B08Z3GRY4K</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>NAN</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>NAN</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>NAN</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>NAN</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>NAN</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
+    <row r="3">
+      <c r="A3" s="8" t="n">
+        <v>44311.60639728075</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>B08Z37PD7L</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
         <is>
           <t>NAN</t>
         </is>
@@ -4253,7 +5453,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4305,7 +5505,7 @@
     </row>
     <row r="2">
       <c r="A2" s="8" t="n">
-        <v>44309.69292205863</v>
+        <v>44311.59799437731</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -4319,7 +5519,7 @@
         <v>1650</v>
       </c>
       <c r="E2" t="n">
-        <v>68308</v>
+        <v>55033</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -4327,7 +5527,7 @@
         </is>
       </c>
       <c r="G2" t="n">
-        <v>284</v>
+        <v>218</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
@@ -4335,205 +5535,35 @@
         </is>
       </c>
     </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:H2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Date</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>ASIN</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>STARS</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>NUM_RATING</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>RANKING1</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>RANKING1_CAT</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>RANKING2</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>RANKING2_CAT</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="8" t="n">
-        <v>44309.69361213892</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>B08Z3CTCCZ</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>NAN</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>NAN</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>NAN</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>NAN</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>NAN</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>NAN</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:H2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Date</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>ASIN</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>STARS</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>NUM_RATING</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>RANKING1</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>RANKING1_CAT</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>RANKING2</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>RANKING2_CAT</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="8" t="n">
-        <v>44309.69362533696</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>B08Z37PD7L</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>NAN</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>NAN</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>NAN</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>NAN</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>NAN</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>NAN</t>
+    <row r="3">
+      <c r="A3" s="8" t="n">
+        <v>44311.60577378672</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>B07WWFWRJP</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>4.4</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1650</v>
+      </c>
+      <c r="E3" t="n">
+        <v>55033</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Home &amp; Kitchen</t>
+        </is>
+      </c>
+      <c r="G3" t="n">
+        <v>218</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Indoor String Lights</t>
         </is>
       </c>
     </row>
@@ -4548,7 +5578,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4600,7 +5630,7 @@
     </row>
     <row r="2">
       <c r="A2" s="8" t="n">
-        <v>44309.69294466566</v>
+        <v>44311.59801424089</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -4633,6 +5663,46 @@
         </is>
       </c>
       <c r="H2" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="8" t="n">
+        <v>44311.60579590865</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>B08Z32GB9S</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
         <is>
           <t>NAN</t>
         </is>
@@ -4649,7 +5719,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4701,7 +5771,7 @@
     </row>
     <row r="2">
       <c r="A2" s="8" t="n">
-        <v>44309.6929583357</v>
+        <v>44311.59802951346</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -4734,6 +5804,46 @@
         </is>
       </c>
       <c r="H2" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="8" t="n">
+        <v>44311.60580798374</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>B08Z3K5QV9</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>NAN</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
         <is>
           <t>NAN</t>
         </is>
@@ -4750,7 +5860,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4802,7 +5912,7 @@
     </row>
     <row r="2">
       <c r="A2" s="8" t="n">
-        <v>44309.6929712211</v>
+        <v>44311.59804231687</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -4816,7 +5926,7 @@
         <v>1003</v>
       </c>
       <c r="E2" t="n">
-        <v>13441</v>
+        <v>10445</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -4824,9 +5934,41 @@
         </is>
       </c>
       <c r="G2" t="n">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="H2" t="inlineStr">
+        <is>
+          <t>Serving Trays</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="8" t="n">
+        <v>44311.60582271108</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>B07R5PCZLY</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>4.7</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1003</v>
+      </c>
+      <c r="E3" t="n">
+        <v>10445</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Kitchen &amp; Dining</t>
+        </is>
+      </c>
+      <c r="G3" t="n">
+        <v>44</v>
+      </c>
+      <c r="H3" t="inlineStr">
         <is>
           <t>Serving Trays</t>
         </is>
@@ -4843,7 +5985,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4895,7 +6037,7 @@
     </row>
     <row r="2">
       <c r="A2" s="8" t="n">
-        <v>44309.69299679068</v>
+        <v>44311.59806522224</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -4909,7 +6051,7 @@
         <v>1003</v>
       </c>
       <c r="E2" t="n">
-        <v>13441</v>
+        <v>10445</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -4917,9 +6059,41 @@
         </is>
       </c>
       <c r="G2" t="n">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="H2" t="inlineStr">
+        <is>
+          <t>Serving Trays</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="8" t="n">
+        <v>44311.60584784326</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>B087QD62HW</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>4.7</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1003</v>
+      </c>
+      <c r="E3" t="n">
+        <v>10445</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Kitchen &amp; Dining</t>
+        </is>
+      </c>
+      <c r="G3" t="n">
+        <v>44</v>
+      </c>
+      <c r="H3" t="inlineStr">
         <is>
           <t>Serving Trays</t>
         </is>
@@ -4936,7 +6110,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4988,7 +6162,7 @@
     </row>
     <row r="2">
       <c r="A2" s="8" t="n">
-        <v>44309.69301749542</v>
+        <v>44311.59808634919</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -5002,7 +6176,7 @@
         <v>237</v>
       </c>
       <c r="E2" t="n">
-        <v>54725</v>
+        <v>73336</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -5010,9 +6184,41 @@
         </is>
       </c>
       <c r="G2" t="n">
-        <v>367</v>
+        <v>554</v>
       </c>
       <c r="H2" t="inlineStr">
+        <is>
+          <t>Serving Trays</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="8" t="n">
+        <v>44311.60586790281</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>B088RG7N5D</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="D3" t="n">
+        <v>237</v>
+      </c>
+      <c r="E3" t="n">
+        <v>73336</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Kitchen &amp; Dining</t>
+        </is>
+      </c>
+      <c r="G3" t="n">
+        <v>554</v>
+      </c>
+      <c r="H3" t="inlineStr">
         <is>
           <t>Serving Trays</t>
         </is>

</xml_diff>